<commit_message>
Nueva metodología. La versión 21 es la final
</commit_message>
<xml_diff>
--- a/version_21/original/tables/Correlaciones.xlsx
+++ b/version_21/original/tables/Correlaciones.xlsx
@@ -403,16 +403,16 @@
         <v>-0.335308770044335</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0140517478070986</v>
+        <v>-0.013072159502638</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.0118030199411789</v>
+        <v>-0.0146574357485768</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.00150662313123837</v>
+        <v>-0.00529308809487509</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00363752462992406</v>
+        <v>0.0264279206184745</v>
       </c>
       <c r="G2" t="n">
         <v>-0.046252885806393</v>
@@ -429,16 +429,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00332555107619491</v>
+        <v>0.00354774033841014</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.00767373541612567</v>
+        <v>-0.00443233804405684</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0278074550419774</v>
+        <v>0.0243516878510086</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00967166320149183</v>
+        <v>0.00932218845596832</v>
       </c>
       <c r="G3" t="n">
         <v>-0.0262121356908608</v>
@@ -449,106 +449,106 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.0140517478070986</v>
+        <v>-0.013072159502638</v>
       </c>
       <c r="B4" t="n">
-        <v>0.00332555107619491</v>
+        <v>0.00354774033841014</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.197264923478256</v>
+        <v>0.175244358258615</v>
       </c>
       <c r="E4" t="n">
-        <v>0.248853600219333</v>
+        <v>0.244521904719147</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0621756833268615</v>
+        <v>0.0788332701121218</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0303557292961098</v>
+        <v>-0.00978788508581947</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.0121538696183547</v>
+        <v>0.0138412561190331</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.0118030199411789</v>
+        <v>-0.0146574357485768</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.00767373541612567</v>
+        <v>-0.00443233804405684</v>
       </c>
       <c r="C5" t="n">
-        <v>0.197264923478256</v>
+        <v>0.175244358258615</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.172568814870545</v>
+        <v>0.160841379848093</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00897079509785812</v>
+        <v>0.0298553915553204</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0887839411897087</v>
+        <v>0.104871857669221</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0101369435180033</v>
+        <v>-0.0159637955996008</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.00150662313123837</v>
+        <v>-0.00529308809487509</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0278074550419774</v>
+        <v>0.0243516878510086</v>
       </c>
       <c r="C6" t="n">
-        <v>0.248853600219333</v>
+        <v>0.244521904719147</v>
       </c>
       <c r="D6" t="n">
-        <v>0.172568814870545</v>
+        <v>0.160841379848093</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.109810297760628</v>
+        <v>0.105045099736656</v>
       </c>
       <c r="G6" t="n">
-        <v>0.124881942334358</v>
+        <v>0.100790758783962</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.0563465991278663</v>
+        <v>-0.0545733735207572</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.00363752462992406</v>
+        <v>0.0264279206184745</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00967166320149183</v>
+        <v>0.00932218845596832</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0621756833268615</v>
+        <v>0.0788332701121218</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00897079509785812</v>
+        <v>0.0298553915553204</v>
       </c>
       <c r="E7" t="n">
-        <v>0.109810297760628</v>
+        <v>0.105045099736656</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0274683143096029</v>
+        <v>-0.0327684638281087</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.00440093185695967</v>
+        <v>0.0132364891612948</v>
       </c>
     </row>
     <row r="8">
@@ -559,16 +559,16 @@
         <v>-0.0262121356908608</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0303557292961098</v>
+        <v>-0.00978788508581947</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0887839411897087</v>
+        <v>0.104871857669221</v>
       </c>
       <c r="E8" t="n">
-        <v>0.124881942334358</v>
+        <v>0.100790758783962</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.0274683143096029</v>
+        <v>-0.0327684638281087</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -585,16 +585,16 @@
         <v>0.0569059977466654</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0121538696183547</v>
+        <v>0.0138412561190331</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0101369435180033</v>
+        <v>-0.0159637955996008</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0563465991278663</v>
+        <v>-0.0545733735207572</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.00440093185695967</v>
+        <v>0.0132364891612948</v>
       </c>
       <c r="G9" t="n">
         <v>-0.332679982222575</v>
@@ -651,16 +651,16 @@
         <v>13364</v>
       </c>
       <c r="C2" t="n">
-        <v>10251</v>
+        <v>10268</v>
       </c>
       <c r="D2" t="n">
-        <v>7586</v>
+        <v>7902</v>
       </c>
       <c r="E2" t="n">
-        <v>8255</v>
+        <v>8289</v>
       </c>
       <c r="F2" t="n">
-        <v>10295</v>
+        <v>10321</v>
       </c>
       <c r="G2" t="n">
         <v>13892</v>
@@ -677,16 +677,16 @@
         <v>13364</v>
       </c>
       <c r="C3" t="n">
-        <v>9848</v>
+        <v>9860</v>
       </c>
       <c r="D3" t="n">
-        <v>7215</v>
+        <v>7518</v>
       </c>
       <c r="E3" t="n">
-        <v>7868</v>
+        <v>7901</v>
       </c>
       <c r="F3" t="n">
-        <v>9842</v>
+        <v>9858</v>
       </c>
       <c r="G3" t="n">
         <v>13364</v>
@@ -697,106 +697,106 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>10251</v>
+        <v>10268</v>
       </c>
       <c r="B4" t="n">
-        <v>9848</v>
+        <v>9860</v>
       </c>
       <c r="C4" t="n">
-        <v>12515</v>
+        <v>12642</v>
       </c>
       <c r="D4" t="n">
-        <v>7395</v>
+        <v>7595</v>
       </c>
       <c r="E4" t="n">
-        <v>7913</v>
+        <v>7903</v>
       </c>
       <c r="F4" t="n">
-        <v>10464</v>
+        <v>10446</v>
       </c>
       <c r="G4" t="n">
-        <v>12515</v>
+        <v>12642</v>
       </c>
       <c r="H4" t="n">
-        <v>12515</v>
+        <v>12642</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7586</v>
+        <v>7902</v>
       </c>
       <c r="B5" t="n">
-        <v>7215</v>
+        <v>7518</v>
       </c>
       <c r="C5" t="n">
-        <v>7395</v>
+        <v>7595</v>
       </c>
       <c r="D5" t="n">
-        <v>8124</v>
+        <v>8477</v>
       </c>
       <c r="E5" t="n">
-        <v>5430</v>
+        <v>5658</v>
       </c>
       <c r="F5" t="n">
-        <v>7226</v>
+        <v>7522</v>
       </c>
       <c r="G5" t="n">
-        <v>8124</v>
+        <v>8477</v>
       </c>
       <c r="H5" t="n">
-        <v>8124</v>
+        <v>8477</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8255</v>
+        <v>8289</v>
       </c>
       <c r="B6" t="n">
-        <v>7868</v>
+        <v>7901</v>
       </c>
       <c r="C6" t="n">
-        <v>7913</v>
+        <v>7903</v>
       </c>
       <c r="D6" t="n">
-        <v>5430</v>
+        <v>5658</v>
       </c>
       <c r="E6" t="n">
-        <v>9159</v>
+        <v>9196</v>
       </c>
       <c r="F6" t="n">
-        <v>8104</v>
+        <v>8143</v>
       </c>
       <c r="G6" t="n">
-        <v>9159</v>
+        <v>9196</v>
       </c>
       <c r="H6" t="n">
-        <v>9159</v>
+        <v>9196</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>10295</v>
+        <v>10321</v>
       </c>
       <c r="B7" t="n">
-        <v>9842</v>
+        <v>9858</v>
       </c>
       <c r="C7" t="n">
-        <v>10464</v>
+        <v>10446</v>
       </c>
       <c r="D7" t="n">
-        <v>7226</v>
+        <v>7522</v>
       </c>
       <c r="E7" t="n">
-        <v>8104</v>
+        <v>8143</v>
       </c>
       <c r="F7" t="n">
-        <v>11994</v>
+        <v>11985</v>
       </c>
       <c r="G7" t="n">
-        <v>11994</v>
+        <v>11985</v>
       </c>
       <c r="H7" t="n">
-        <v>11994</v>
+        <v>11985</v>
       </c>
     </row>
     <row r="8">
@@ -807,16 +807,16 @@
         <v>13364</v>
       </c>
       <c r="C8" t="n">
-        <v>12515</v>
+        <v>12642</v>
       </c>
       <c r="D8" t="n">
-        <v>8124</v>
+        <v>8477</v>
       </c>
       <c r="E8" t="n">
-        <v>9159</v>
+        <v>9196</v>
       </c>
       <c r="F8" t="n">
-        <v>11994</v>
+        <v>11985</v>
       </c>
       <c r="G8" t="n">
         <v>17045</v>
@@ -833,16 +833,16 @@
         <v>13347</v>
       </c>
       <c r="C9" t="n">
-        <v>12515</v>
+        <v>12642</v>
       </c>
       <c r="D9" t="n">
-        <v>8124</v>
+        <v>8477</v>
       </c>
       <c r="E9" t="n">
-        <v>9159</v>
+        <v>9196</v>
       </c>
       <c r="F9" t="n">
-        <v>11994</v>
+        <v>11985</v>
       </c>
       <c r="G9" t="n">
         <v>17006</v>
@@ -897,16 +897,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.154852965564903</v>
+        <v>0.185333010147666</v>
       </c>
       <c r="D2" t="n">
-        <v>0.304005501758686</v>
+        <v>0.192639588593982</v>
       </c>
       <c r="E2" t="n">
-        <v>0.891136198462688</v>
+        <v>0.629923645952377</v>
       </c>
       <c r="F2" t="n">
-        <v>0.712101472308993</v>
+        <v>0.00725259927634214</v>
       </c>
       <c r="G2" t="n">
         <v>0.0000000492509750760206</v>
@@ -921,16 +921,16 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="n">
-        <v>0.741417316952506</v>
+        <v>0.724659550264867</v>
       </c>
       <c r="D3" t="n">
-        <v>0.514586582314783</v>
+        <v>0.700793115246161</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0136381723046801</v>
+        <v>0.0304228670195137</v>
       </c>
       <c r="F3" t="n">
-        <v>0.337359363925908</v>
+        <v>0.35471671706527</v>
       </c>
       <c r="G3" t="n">
         <v>0.00244203648127295</v>
@@ -941,10 +941,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.154852965564903</v>
+        <v>0.185333010147666</v>
       </c>
       <c r="B4" t="n">
-        <v>0.741417316952506</v>
+        <v>0.724659550264867</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="n">
@@ -954,21 +954,21 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.000000000194553706478473</v>
+        <v>0.000000000000000666133814775094</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00068290264669324</v>
+        <v>0.27114283846555</v>
       </c>
       <c r="H4" t="n">
-        <v>0.173964961740664</v>
+        <v>0.119664081876168</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.304005501758686</v>
+        <v>0.192639588593982</v>
       </c>
       <c r="B5" t="n">
-        <v>0.514586582314783</v>
+        <v>0.700793115246161</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -978,21 +978,21 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.445789227081683</v>
+        <v>0.00961184991791564</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00000000000000111022302462516</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.360948940928618</v>
+        <v>0.141650194161857</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.891136198462688</v>
+        <v>0.629923645952377</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0136381723046801</v>
+        <v>0.0304228670195137</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1008,31 +1008,31 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0000000681161034243871</v>
+        <v>0.000000163608588898967</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.712101472308993</v>
+        <v>0.00725259927634214</v>
       </c>
       <c r="B7" t="n">
-        <v>0.337359363925908</v>
+        <v>0.35471671706527</v>
       </c>
       <c r="C7" t="n">
-        <v>0.000000000194553706478473</v>
+        <v>0.000000000000000666133814775094</v>
       </c>
       <c r="D7" t="n">
-        <v>0.445789227081683</v>
+        <v>0.00961184991791564</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.00262536645169309</v>
+        <v>0.000333287597972021</v>
       </c>
       <c r="H7" t="n">
-        <v>0.629856035454258</v>
+        <v>0.147340223147381</v>
       </c>
     </row>
     <row r="8">
@@ -1043,16 +1043,16 @@
         <v>0.00244203648127295</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00068290264669324</v>
+        <v>0.27114283846555</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00000000000000111022302462516</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00262536645169309</v>
+        <v>0.000333287597972021</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="n">
@@ -1067,16 +1067,16 @@
         <v>0.0000000000473556749369664</v>
       </c>
       <c r="C9" t="n">
-        <v>0.173964961740664</v>
+        <v>0.119664081876168</v>
       </c>
       <c r="D9" t="n">
-        <v>0.360948940928618</v>
+        <v>0.141650194161857</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0000000681161034243871</v>
+        <v>0.000000163608588898967</v>
       </c>
       <c r="F9" t="n">
-        <v>0.629856035454258</v>
+        <v>0.147340223147381</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>

</xml_diff>